<commit_message>
Updated files from latest code for documentation
</commit_message>
<xml_diff>
--- a/CatalogData.xlsx
+++ b/CatalogData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,36 +20,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">Key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://staging.unityinfluence.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adminUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://api-staging.unityinfluence.com/admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adminEmail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">development@unityinfluence.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adminPassword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unityinfluence</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+  <si>
+    <t xml:space="preserve">invalidUsername</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalidPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectedErrorLocator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectedErrorMessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validUsername</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectedPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parul93@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$("[class*='error']")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorry! The login credentials are not valid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parul.adhikari+staff@quovantis.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content-requests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parul.adhikari+am@quovantis.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parul.adhikari+noaccess@quovantis.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unauthorized access.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parul.adhikari+photo@quovantis.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre-production-board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parul Adhikari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parul.adhikari+managed@quovantis.com</t>
   </si>
 </sst>
 </file>
@@ -59,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -80,6 +107,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,13 +164,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -150,58 +206,152 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.6683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.780612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.1989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B2" s="3" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="parul93@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId2" display="parul.adhikari+staff@quovantis.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="parul.adhikari+staff@quovantis.com"/>
+    <hyperlink ref="E3" r:id="rId4" display="parul.adhikari+am@quovantis.com"/>
+    <hyperlink ref="A4" r:id="rId5" display="parul.adhikari+noaccess@quovantis.com"/>
+    <hyperlink ref="E4" r:id="rId6" display="parul.adhikari+photo@quovantis.com"/>
+    <hyperlink ref="E5" r:id="rId7" display="parul.adhikari+managed@quovantis.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>